<commit_message>
add new structs and enums
</commit_message>
<xml_diff>
--- a/vd/NEC Table 9 data.xlsx
+++ b/vd/NEC Table 9 data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ma.wright\dev\feeders-rust\vd\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattw\dev\feeders-rust\vd\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEDDB58-5DB6-44F2-A8E3-AE3759F0EFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="825" yWindow="7485" windowWidth="30585" windowHeight="23025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEC Table 9 data" sheetId="1" r:id="rId1"/>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
   <si>
     <t>00</t>
   </si>
@@ -47,9 +48,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>CU</t>
-  </si>
-  <si>
     <t>R/CU</t>
   </si>
   <si>
@@ -65,7 +63,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -882,11 +880,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,10 +893,9 @@
     <col min="5" max="5" width="2.7109375" customWidth="1"/>
     <col min="9" max="9" width="2.7109375" customWidth="1"/>
     <col min="13" max="13" width="2.7109375" customWidth="1"/>
-    <col min="17" max="17" width="2.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
         <v>7</v>
       </c>
@@ -907,46 +904,27 @@
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="M1" s="3"/>
-      <c r="N1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S1" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
@@ -974,27 +952,8 @@
         <v>4</v>
       </c>
       <c r="M2" s="3"/>
-      <c r="N2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>14</v>
       </c>
@@ -1026,27 +985,8 @@
         <v>0</v>
       </c>
       <c r="M3" s="2"/>
-      <c r="N3" s="2">
-        <v>2.7</v>
-      </c>
-      <c r="O3" s="2">
-        <v>2.7</v>
-      </c>
-      <c r="P3" s="2">
-        <v>2.7</v>
-      </c>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="4">
-        <v>0</v>
-      </c>
-      <c r="S3" s="4">
-        <v>0</v>
-      </c>
-      <c r="T3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12</v>
       </c>
@@ -1078,27 +1018,8 @@
         <v>3.2</v>
       </c>
       <c r="M4" s="2"/>
-      <c r="N4" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="O4" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="P4" s="2">
-        <v>1.7</v>
-      </c>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="S4" s="2">
-        <v>2.8</v>
-      </c>
-      <c r="T4" s="2">
-        <v>2.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>10</v>
       </c>
@@ -1130,27 +1051,8 @@
         <v>2</v>
       </c>
       <c r="M5" s="2"/>
-      <c r="N5" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="O5" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="P5" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="S5" s="2">
-        <v>1.8</v>
-      </c>
-      <c r="T5" s="2">
-        <v>1.8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>8</v>
       </c>
@@ -1182,27 +1084,8 @@
         <v>1.3</v>
       </c>
       <c r="M6" s="2"/>
-      <c r="N6" s="2">
-        <v>0.69</v>
-      </c>
-      <c r="O6" s="2">
-        <v>0.69</v>
-      </c>
-      <c r="P6" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="S6" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="T6" s="2">
-        <v>1.1000000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1234,27 +1117,8 @@
         <v>0.81</v>
       </c>
       <c r="M7" s="2"/>
-      <c r="N7" s="2">
-        <v>0.44</v>
-      </c>
-      <c r="O7" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="P7" s="2">
-        <v>0.45</v>
-      </c>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2">
-        <v>0.71</v>
-      </c>
-      <c r="S7" s="2">
-        <v>0.72</v>
-      </c>
-      <c r="T7" s="2">
-        <v>0.72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>4</v>
       </c>
@@ -1286,27 +1150,8 @@
         <v>0.51</v>
       </c>
       <c r="M8" s="2"/>
-      <c r="N8" s="2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="O8" s="2">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="P8" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="S8" s="2">
-        <v>0.46</v>
-      </c>
-      <c r="T8" s="2">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>3</v>
       </c>
@@ -1338,27 +1183,8 @@
         <v>0.4</v>
       </c>
       <c r="M9" s="2"/>
-      <c r="N9" s="2">
-        <v>0.23</v>
-      </c>
-      <c r="O9" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="P9" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="S9" s="2">
-        <v>0.37</v>
-      </c>
-      <c r="T9" s="2">
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>2</v>
       </c>
@@ -1390,27 +1216,8 @@
         <v>0.32</v>
       </c>
       <c r="M10" s="2"/>
-      <c r="N10" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="O10" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="P10" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="S10" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="T10" s="2">
-        <v>0.3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>1</v>
       </c>
@@ -1442,27 +1249,8 @@
         <v>0.25</v>
       </c>
       <c r="M11" s="2"/>
-      <c r="N11" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="O11" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="P11" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="S11" s="2">
-        <v>0.24</v>
-      </c>
-      <c r="T11" s="2">
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>0</v>
       </c>
@@ -1494,27 +1282,8 @@
         <v>0.2</v>
       </c>
       <c r="M12" s="2"/>
-      <c r="N12" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="O12" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="P12" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="Q12" s="2"/>
-      <c r="R12" s="2">
-        <v>0.19</v>
-      </c>
-      <c r="S12" s="2">
-        <v>0.2</v>
-      </c>
-      <c r="T12" s="2">
-        <v>0.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
@@ -1546,27 +1315,8 @@
         <v>0.16</v>
       </c>
       <c r="M13" s="2"/>
-      <c r="N13" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="O13" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="P13" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="Q13" s="2"/>
-      <c r="R13" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="S13" s="2">
-        <v>0.16</v>
-      </c>
-      <c r="T13" s="2">
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1598,27 +1348,8 @@
         <v>0.13</v>
       </c>
       <c r="M14" s="2"/>
-      <c r="N14" s="2">
-        <v>8.7999999999999995E-2</v>
-      </c>
-      <c r="O14" s="2">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="P14" s="2">
-        <v>9.4E-2</v>
-      </c>
-      <c r="Q14" s="2"/>
-      <c r="R14" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="S14" s="2">
-        <v>0.13</v>
-      </c>
-      <c r="T14" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>2</v>
       </c>
@@ -1650,27 +1381,8 @@
         <v>0.1</v>
       </c>
       <c r="M15" s="2"/>
-      <c r="N15" s="2">
-        <v>7.3999999999999996E-2</v>
-      </c>
-      <c r="O15" s="2">
-        <v>7.8E-2</v>
-      </c>
-      <c r="P15" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="Q15" s="2"/>
-      <c r="R15" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="S15" s="2">
-        <v>0.11</v>
-      </c>
-      <c r="T15" s="2">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>250</v>
       </c>
@@ -1702,27 +1414,8 @@
         <v>8.5999999999999993E-2</v>
       </c>
       <c r="M16" s="2"/>
-      <c r="N16" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="O16" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="P16" s="2">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="Q16" s="2"/>
-      <c r="R16" s="2">
-        <v>9.4E-2</v>
-      </c>
-      <c r="S16" s="2">
-        <v>9.8000000000000004E-2</v>
-      </c>
-      <c r="T16" s="2">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>300</v>
       </c>
@@ -1754,27 +1447,8 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="M17" s="2"/>
-      <c r="N17" s="2">
-        <v>5.8999999999999997E-2</v>
-      </c>
-      <c r="O17" s="2">
-        <v>6.3E-2</v>
-      </c>
-      <c r="P17" s="2">
-        <v>6.5000000000000002E-2</v>
-      </c>
-      <c r="Q17" s="2"/>
-      <c r="R17" s="2">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="S17" s="2">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="T17" s="2">
-        <v>8.7999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>350</v>
       </c>
@@ -1806,27 +1480,8 @@
         <v>6.3E-2</v>
       </c>
       <c r="M18" s="2"/>
-      <c r="N18" s="2">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="O18" s="2">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="P18" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="Q18" s="2"/>
-      <c r="R18" s="2">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="S18" s="2">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="T18" s="2">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>400</v>
       </c>
@@ -1858,27 +1513,8 @@
         <v>5.5E-2</v>
       </c>
       <c r="M19" s="2"/>
-      <c r="N19" s="2">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="O19" s="2">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="P19" s="2">
-        <v>5.6000000000000001E-2</v>
-      </c>
-      <c r="Q19" s="2"/>
-      <c r="R19" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="S19" s="2">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="T19" s="2">
-        <v>7.2999999999999995E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>500</v>
       </c>
@@ -1910,27 +1546,8 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="M20" s="2"/>
-      <c r="N20" s="2">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="O20" s="2">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="P20" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="Q20" s="2"/>
-      <c r="R20" s="2">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="S20" s="2">
-        <v>6.0999999999999999E-2</v>
-      </c>
-      <c r="T20" s="2">
-        <v>6.4000000000000001E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>600</v>
       </c>
@@ -1962,27 +1579,8 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="M21" s="2"/>
-      <c r="N21" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="O21" s="2">
-        <v>4.3999999999999997E-2</v>
-      </c>
-      <c r="P21" s="2">
-        <v>4.7E-2</v>
-      </c>
-      <c r="Q21" s="2"/>
-      <c r="R21" s="2">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="S21" s="2">
-        <v>5.5E-2</v>
-      </c>
-      <c r="T21" s="2">
-        <v>5.8000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>750</v>
       </c>
@@ -2014,27 +1612,8 @@
         <v>3.1E-2</v>
       </c>
       <c r="M22" s="2"/>
-      <c r="N22" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="O22" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="P22" s="2">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="Q22" s="2"/>
-      <c r="R22" s="2">
-        <v>4.4999999999999998E-2</v>
-      </c>
-      <c r="S22" s="2">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="T22" s="2">
-        <v>5.1999999999999998E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>1000</v>
       </c>
@@ -2066,34 +1645,15 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="M23" s="2"/>
-      <c r="N23" s="2">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="O23" s="2">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="P23" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="Q23" s="2"/>
-      <c r="R23" s="2">
-        <v>3.9E-2</v>
-      </c>
-      <c r="S23" s="2">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="T23" s="2">
-        <v>4.5999999999999999E-2</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -2103,7 +1663,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2115,7 +1675,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
add data for tables
</commit_message>
<xml_diff>
--- a/vd/NEC Table 9 data.xlsx
+++ b/vd/NEC Table 9 data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23624"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattw\dev\feeders-rust\vd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AEDDB58-5DB6-44F2-A8E3-AE3759F0EFF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAE94D76-69C2-4BEA-B741-8CACCCF8DDBC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="825" yWindow="7485" windowWidth="30585" windowHeight="23025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22800" yWindow="10440" windowWidth="33030" windowHeight="23295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NEC Table 9 data" sheetId="1" r:id="rId1"/>
@@ -22,16 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="12">
-  <si>
-    <t>00</t>
-  </si>
-  <si>
-    <t>000</t>
-  </si>
-  <si>
-    <t>0000</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>PVC/AL</t>
   </si>
@@ -58,6 +49,18 @@
   </si>
   <si>
     <t>http://profwagner.com/4520/4520-PPT10.pdf</t>
+  </si>
+  <si>
+    <t>1/0</t>
+  </si>
+  <si>
+    <t>2/0</t>
+  </si>
+  <si>
+    <t>3/0</t>
+  </si>
+  <si>
+    <t>4/0</t>
   </si>
 </sst>
 </file>
@@ -883,8 +886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -897,59 +900,59 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C1" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="E1" s="3"/>
       <c r="F1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I1" s="3"/>
       <c r="J1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="L1" s="3" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="M1" s="3"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C2" s="3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E2" s="3"/>
       <c r="F2" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I2" s="3"/>
       <c r="J2" s="3" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="M2" s="3"/>
     </row>
@@ -1251,8 +1254,8 @@
       <c r="M11" s="2"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1">
-        <v>0</v>
+      <c r="A12" s="1" t="s">
+        <v>9</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="2">
@@ -1285,7 +1288,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="2">
@@ -1318,7 +1321,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="2">
@@ -1351,7 +1354,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="2">
@@ -1648,12 +1651,12 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>